<commit_message>
Update STM32 Flight Controller.xlsx
</commit_message>
<xml_diff>
--- a/STM32 Flight Controller/STM32 Flight Controller.xlsx
+++ b/STM32 Flight Controller/STM32 Flight Controller.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Users\fores\Documents\GitHub\Aruino-Drone\STM32 Flight Controller\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\fores\Documents\GitHub\Aruino-Drone\STM32 Flight Controller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA7F360D-B3E9-4983-932E-0DE91106EF0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2EFF0B5C-24C1-470B-9FEC-0800F9C48BA6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" xr2:uid="{0A21A7E5-692B-4F54-8B90-96DCD7BDE2FE}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{0A21A7E5-692B-4F54-8B90-96DCD7BDE2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="STM32 Flight Controller" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -428,8 +428,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -445,6 +452,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
   </fills>
@@ -472,20 +484,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" quotePrefix="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="2" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Bad" xfId="2" builtinId="27"/>
     <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -802,7 +816,7 @@
   <dimension ref="A1:F34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F30" sqref="F30"/>
+      <selection activeCell="H23" sqref="H23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -811,641 +825,641 @@
     <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:6" s="2" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" s="1">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1">
-        <v>1</v>
-      </c>
-      <c r="F3" s="2" t="s">
+      <c r="E3" s="4">
+        <v>1</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E4" s="1">
+      <c r="E4" s="4">
         <v>2</v>
       </c>
-      <c r="F4" s="2" t="s">
+      <c r="F4" s="3" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="2" t="s">
+      <c r="D5" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="1">
+      <c r="E5" s="4">
         <v>3</v>
       </c>
-      <c r="F5" s="2" t="s">
+      <c r="F5" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="E6" s="1">
+      <c r="E6" s="6">
         <v>2</v>
       </c>
-      <c r="F6" s="2" t="s">
+      <c r="F6" s="5" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="6">
         <v>2</v>
       </c>
-      <c r="F7" s="2" t="s">
+      <c r="F7" s="5" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E8" s="1">
-        <v>1</v>
-      </c>
-      <c r="F8" s="1"/>
+      <c r="E8" s="6">
+        <v>1</v>
+      </c>
+      <c r="F8" s="6"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="E9" s="1">
+      <c r="E9" s="6">
         <v>4</v>
       </c>
-      <c r="F9" s="1"/>
+      <c r="F9" s="6"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E10" s="1">
+      <c r="E10" s="4">
         <v>2</v>
       </c>
-      <c r="F10" s="1"/>
+      <c r="F10" s="4"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
+      <c r="A11" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="C11" s="5" t="s">
+      <c r="C11" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="E11" s="6">
-        <v>1</v>
-      </c>
-      <c r="F11" s="6"/>
+      <c r="E11" s="4">
+        <v>1</v>
+      </c>
+      <c r="F11" s="4"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="1"/>
+      <c r="E12" s="6">
+        <v>1</v>
+      </c>
+      <c r="F12" s="6"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="5" t="s">
+      <c r="A13" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="5" t="s">
+      <c r="B13" s="4"/>
+      <c r="C13" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="E13" s="6">
-        <v>1</v>
-      </c>
-      <c r="F13" s="6"/>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="4"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C14" s="2" t="s">
+      <c r="C14" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="D14" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="E14" s="1">
-        <v>1</v>
-      </c>
-      <c r="F14" s="1"/>
+      <c r="E14" s="4">
+        <v>1</v>
+      </c>
+      <c r="F14" s="4"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
+      <c r="A15" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="B15" s="2" t="s">
+      <c r="B15" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="C15" s="2" t="s">
+      <c r="C15" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="D15" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="E15" s="1">
-        <v>1</v>
-      </c>
-      <c r="F15" s="1"/>
+      <c r="E15" s="6">
+        <v>1</v>
+      </c>
+      <c r="F15" s="6"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="C16" s="2" t="s">
+      <c r="C16" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="D16" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E16" s="1">
-        <v>1</v>
-      </c>
-      <c r="F16" s="1"/>
+      <c r="E16" s="6">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
+      <c r="A17" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="5" t="s">
         <v>61</v>
       </c>
-      <c r="C17" s="2" t="s">
+      <c r="C17" s="5" t="s">
         <v>62</v>
       </c>
-      <c r="D17" s="2" t="s">
+      <c r="D17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="1"/>
+      <c r="E17" s="6">
+        <v>1</v>
+      </c>
+      <c r="F17" s="6"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+      <c r="A18" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B18" s="5" t="s">
+      <c r="B18" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C18" s="5" t="s">
+      <c r="C18" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="E18" s="6">
+      <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="F18" s="6"/>
+      <c r="F18" s="4"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2" t="s">
+      <c r="A19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="5" t="s">
         <v>67</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="C19" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="D19" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="E19" s="1">
+      <c r="E19" s="6">
         <v>2</v>
       </c>
-      <c r="F19" s="1"/>
+      <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
+      <c r="A20" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="C20" s="2" t="s">
+      <c r="C20" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="D20" s="2" t="s">
+      <c r="D20" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="E20" s="1">
-        <v>1</v>
-      </c>
-      <c r="F20" s="1"/>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="C21" s="2" t="s">
+      <c r="C21" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="D21" s="2" t="s">
+      <c r="D21" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="E21" s="1">
-        <v>1</v>
-      </c>
-      <c r="F21" s="1"/>
+      <c r="E21" s="4">
+        <v>1</v>
+      </c>
+      <c r="F21" s="4"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="2" t="s">
+      <c r="A22" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B22" s="2" t="s">
+      <c r="B22" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D22" s="2" t="s">
+      <c r="D22" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E22" s="1">
-        <v>1</v>
-      </c>
-      <c r="F22" s="1"/>
+      <c r="E22" s="4">
+        <v>1</v>
+      </c>
+      <c r="F22" s="4"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="2" t="s">
+      <c r="A23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="2" t="s">
+      <c r="C23" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="D23" s="2" t="s">
+      <c r="D23" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="E23" s="1">
-        <v>1</v>
-      </c>
-      <c r="F23" s="1"/>
+      <c r="E23" s="4">
+        <v>1</v>
+      </c>
+      <c r="F23" s="4"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+      <c r="A24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B24" s="5" t="s">
+      <c r="B24" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="C24" s="5" t="s">
+      <c r="C24" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="E24" s="6">
-        <v>1</v>
-      </c>
-      <c r="F24" s="6"/>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C25" s="2" t="s">
+      <c r="C25" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="D25" s="2" t="s">
+      <c r="D25" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="E25" s="1">
+      <c r="E25" s="6">
         <v>2</v>
       </c>
-      <c r="F25" s="1"/>
+      <c r="F25" s="6"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C26" s="2" t="s">
+      <c r="C26" s="3" t="s">
         <v>95</v>
       </c>
-      <c r="D26" s="2" t="s">
+      <c r="D26" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E26" s="1">
-        <v>1</v>
-      </c>
-      <c r="F26" s="2" t="s">
+      <c r="E26" s="4">
+        <v>1</v>
+      </c>
+      <c r="F26" s="3" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+      <c r="A27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B27" s="5" t="s">
+      <c r="B27" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C27" s="5" t="s">
+      <c r="C27" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E27" s="6">
+      <c r="E27" s="4">
         <v>6</v>
       </c>
-      <c r="F27" s="5" t="s">
+      <c r="F27" s="3" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
+      <c r="A28" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B28" s="5" t="s">
+      <c r="B28" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E28" s="6">
+      <c r="E28" s="4">
         <v>3</v>
       </c>
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="3" t="s">
         <v>100</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
+      <c r="A29" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="C29" s="2" t="s">
+      <c r="C29" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="D29" s="2" t="s">
+      <c r="D29" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="E29" s="1">
+      <c r="E29" s="4">
         <v>3</v>
       </c>
-      <c r="F29" s="2" t="s">
+      <c r="F29" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
+      <c r="A30" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C30" s="2" t="s">
+      <c r="C30" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="D30" s="2" t="s">
+      <c r="D30" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="E30" s="1">
-        <v>1</v>
-      </c>
-      <c r="F30" s="2" t="s">
+      <c r="E30" s="6">
+        <v>1</v>
+      </c>
+      <c r="F30" s="5" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="C31" s="2" t="s">
+      <c r="C31" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="2" t="s">
+      <c r="D31" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="E31" s="1">
-        <v>1</v>
-      </c>
-      <c r="F31" s="2" t="s">
+      <c r="E31" s="4">
+        <v>1</v>
+      </c>
+      <c r="F31" s="3" t="s">
         <v>112</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="2" t="s">
+      <c r="A32" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D32" s="2" t="s">
+      <c r="D32" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="E32" s="1">
-        <v>1</v>
-      </c>
-      <c r="F32" s="1"/>
+      <c r="E32" s="6">
+        <v>1</v>
+      </c>
+      <c r="F32" s="6"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B33" s="5" t="s">
+      <c r="B33" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C33" s="5" t="s">
+      <c r="C33" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="E33" s="6">
-        <v>1</v>
-      </c>
-      <c r="F33" s="6"/>
+      <c r="E33" s="4">
+        <v>1</v>
+      </c>
+      <c r="F33" s="4"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+      <c r="A34" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="B34" s="5" t="s">
+      <c r="B34" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="C34" s="5" t="s">
+      <c r="C34" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="E34" s="6">
+      <c r="E34" s="4">
         <v>5</v>
       </c>
-      <c r="F34" s="6"/>
+      <c r="F34" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>